<commit_message>
chore: version update to 0.8.4 #75
</commit_message>
<xml_diff>
--- a/support/docs/specifications/ahc-hrsn-elt/screening/1115-Hub FHIR Mapping.xlsx
+++ b/support/docs/specifications/ahc-hrsn-elt/screening/1115-Hub FHIR Mapping.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27514"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53DA9E24-12CA-4141-A802-25206FB8700D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B657C39-33A4-4028-9F64-ED7937B2410F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="706" firstSheet="5" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="706" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="10" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="290">
   <si>
     <t>Genaral Comments</t>
   </si>
@@ -69,13 +69,16 @@
     <t>Mapping logic to get the required data from the source data fields.</t>
   </si>
   <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>The field is updated in the 1115-hub release version</t>
+  </si>
+  <si>
     <t>QCS Feedback</t>
   </si>
   <si>
     <t>Comments based on the review</t>
-  </si>
-  <si>
-    <t>Version</t>
   </si>
   <si>
     <t>NYeC/Ready/Slalom Feedback</t>
@@ -307,6 +310,9 @@
     <t xml:space="preserve">MR- for PAT MRN ID, add MA for MEDICAID_CIN </t>
   </si>
   <si>
+    <t xml:space="preserve">Yes and PN for MPIID. </t>
+  </si>
+  <si>
     <t>identifier.type</t>
   </si>
   <si>
@@ -331,6 +337,9 @@
     <t>http://www.sacredheart.gov/facility/CUMC</t>
   </si>
   <si>
+    <t xml:space="preserve">This will be updated to SCN in new CSVs. </t>
+  </si>
+  <si>
     <t>identifier.value</t>
   </si>
   <si>
@@ -349,6 +358,9 @@
     <t>Organization ID is not there in the data directly, please clarify from where we will get the Organization ID</t>
   </si>
   <si>
+    <t>Organization ID should be Facility ID.</t>
+  </si>
+  <si>
     <t>MA</t>
   </si>
   <si>
@@ -367,6 +379,9 @@
     <t>in SHINNY IG the code seems PN, but in ticket #69 its NP. Please clarify. this release we updated as PN</t>
   </si>
   <si>
+    <t xml:space="preserve">Should be PN not NP. </t>
+  </si>
+  <si>
     <t>active</t>
   </si>
   <si>
@@ -697,6 +712,9 @@
     <t>http://shinny.org/StructureDefinition/shin-ny-organization</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>generated</t>
   </si>
   <si>
@@ -706,6 +724,9 @@
     <t>Field not available to select these values draft | proposed | active | rejected | inactive | entered-in-error</t>
   </si>
   <si>
+    <t>Use active</t>
+  </si>
+  <si>
     <t>scope</t>
   </si>
   <si>
@@ -721,6 +742,9 @@
     <t xml:space="preserve">Field not available to select these values Advanced Care Directive | Research | Privacy Consent | Treatment	</t>
   </si>
   <si>
+    <t>Use treatment</t>
+  </si>
+  <si>
     <t>scope.text</t>
   </si>
   <si>
@@ -742,6 +766,9 @@
     <t>patient/&lt;Patient ID&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">Slalom has reference as patient name JonDoe. But I think this Patient ID works. </t>
+  </si>
+  <si>
     <t>dateTime</t>
   </si>
   <si>
@@ -769,12 +796,18 @@
     <t xml:space="preserve">Organization ID is not there in the data directly, please clarify from where we will get the Organization ID, Is it QE_ADMIN_DATA.facilityId </t>
   </si>
   <si>
+    <t>Use facility ID</t>
+  </si>
+  <si>
     <t>meta</t>
   </si>
   <si>
     <t>met.profile</t>
   </si>
   <si>
+    <t>Yes use this</t>
+  </si>
+  <si>
     <t>Optional. Not given.</t>
   </si>
   <si>
@@ -872,13 +905,16 @@
   </si>
   <si>
     <t>finished</t>
+  </si>
+  <si>
+    <t>I think your patient ID works just want to keep this consistent. The logical id of the resource, as used in the URL for the resource. Once assigned, this value never changes.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -931,6 +967,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -997,7 +1041,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1029,10 +1073,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1042,13 +1092,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1358,10 +1406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D4FEC9-B81F-4F1A-91E6-6DEE9CDF6748}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1372,38 +1420,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:11" ht="60" customHeight="1">
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17"/>
+      <c r="C2" s="21"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="17"/>
+      <c r="C3" s="21"/>
     </row>
     <row r="4" spans="1:11" ht="30" customHeight="1">
       <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="21"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
       <c r="A5" s="6"/>
@@ -1432,7 +1480,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1">
+    <row r="8" spans="1:11">
       <c r="A8" s="6"/>
       <c r="B8" s="5" t="s">
         <v>10</v>
@@ -1443,17 +1491,21 @@
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
       <c r="A9" s="6"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="B9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
       <c r="A10" s="6"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1">
       <c r="A11" s="6"/>
@@ -1469,6 +1521,11 @@
       <c r="A13" s="6"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1">
+      <c r="A14" s="6"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1485,15 +1542,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.5703125" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="4" width="41.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="52.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="88.140625" customWidth="1"/>
     <col min="7" max="7" width="51.7109375" customWidth="1"/>
@@ -1511,117 +1569,117 @@
         <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="60.75">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -1629,57 +1687,57 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C15"/>
       <c r="D15"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1692,17 +1750,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:E7"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="53.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="4" width="60.28515625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="50.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="55.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="66.42578125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="46.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="48" customWidth="1"/>
     <col min="7" max="7" width="51.7109375" customWidth="1"/>
     <col min="8" max="8" width="25.85546875" customWidth="1"/>
   </cols>
@@ -1718,188 +1777,188 @@
         <v>8</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>46</v>
+      <c r="C4" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30.75">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>47</v>
+      <c r="C5" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>25</v>
+      <c r="C7" s="22" t="s">
+        <v>26</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="45.75">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D14" s="10"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.5" customHeight="1">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1908,63 +1967,63 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D21" s="10"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17.25" customHeight="1">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17.25" customHeight="1">
@@ -1973,24 +2032,24 @@
     </row>
     <row r="27" spans="1:4" ht="17.25" customHeight="1">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17.25" customHeight="1">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17.25" customHeight="1">
@@ -1999,482 +2058,482 @@
     </row>
     <row r="30" spans="1:4" ht="17.25" customHeight="1">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>89</v>
+      </c>
+      <c r="F36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>97</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F41" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="30.75">
+      <c r="A44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="11" t="s">
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
         <v>92</v>
       </c>
-      <c r="D39" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" t="s">
+      <c r="C46" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
         <v>93</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C47" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="16.5">
+      <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D40" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" t="s">
+      <c r="D54" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="30.75">
+      <c r="A55" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F55" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
         <v>95</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" t="s">
+      <c r="D56" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
         <v>97</v>
       </c>
-      <c r="C42" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="30.75">
-      <c r="A44" t="s">
+      <c r="C57" s="23"/>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
         <v>100</v>
       </c>
-      <c r="C44" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44" s="1" t="s">
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
-      <c r="A45" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" s="12" t="s">
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
         <v>103</v>
       </c>
-      <c r="D47" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" t="s">
-        <v>100</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" t="s">
-        <v>90</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="30.75">
-      <c r="A55" t="s">
-        <v>91</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" t="s">
-        <v>93</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" t="s">
-        <v>95</v>
-      </c>
-      <c r="C57" s="13"/>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" t="s">
-        <v>100</v>
-      </c>
       <c r="C60" s="12" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C62" s="12" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="45.75">
+    <row r="63" spans="1:6" ht="30.75">
       <c r="A63" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="30.75">
       <c r="A65" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B65" t="s">
         <v>6</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>116</v>
-      </c>
-      <c r="C66" s="10"/>
+        <v>121</v>
+      </c>
       <c r="D66" s="10"/>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>117</v>
-      </c>
-      <c r="C67" s="10"/>
+        <v>122</v>
+      </c>
       <c r="D67" s="10"/>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>118</v>
-      </c>
-      <c r="C68" s="10"/>
+        <v>123</v>
+      </c>
       <c r="D68" s="10"/>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>119</v>
-      </c>
-      <c r="C69" s="10"/>
+        <v>124</v>
+      </c>
       <c r="D69" s="10"/>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>120</v>
-      </c>
-      <c r="C70" s="10"/>
+        <v>125</v>
+      </c>
       <c r="D70" s="10"/>
     </row>
     <row r="71" spans="1:5">
-      <c r="C71" s="10"/>
       <c r="D71" s="10"/>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B72" t="s">
         <v>6</v>
       </c>
-      <c r="C72" s="10" t="s">
-        <v>122</v>
+      <c r="C72" s="12" t="s">
+        <v>127</v>
       </c>
       <c r="D72" s="10"/>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>123</v>
-      </c>
-      <c r="C73" s="10" t="s">
-        <v>124</v>
+        <v>128</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>129</v>
       </c>
       <c r="D73" s="10"/>
     </row>
     <row r="74" spans="1:5">
-      <c r="C74" s="10"/>
       <c r="D74" s="10"/>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>125</v>
-      </c>
-      <c r="C75" s="10"/>
+        <v>130</v>
+      </c>
       <c r="D75" s="10"/>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>126</v>
-      </c>
-      <c r="C76" s="10" t="s">
-        <v>127</v>
+        <v>131</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>132</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>128</v>
-      </c>
-      <c r="C77" s="10" t="s">
-        <v>129</v>
+        <v>133</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>134</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>130</v>
-      </c>
-      <c r="C78" s="10" t="s">
-        <v>131</v>
+        <v>135</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>136</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>132</v>
-      </c>
-      <c r="C79" s="10" t="s">
-        <v>133</v>
+        <v>137</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>130</v>
-      </c>
-      <c r="C80" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>139</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E80"/>
     </row>
     <row r="81" spans="1:5">
-      <c r="C81" s="10"/>
       <c r="D81" s="10"/>
       <c r="E81"/>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>135</v>
-      </c>
-      <c r="C82" s="10"/>
+        <v>140</v>
+      </c>
       <c r="D82" s="10"/>
       <c r="E82"/>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>136</v>
-      </c>
-      <c r="C83" s="10"/>
+        <v>141</v>
+      </c>
       <c r="D83" s="10"/>
       <c r="E83"/>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B84" t="s">
-        <v>138</v>
-      </c>
-      <c r="C84" s="10"/>
+        <v>143</v>
+      </c>
       <c r="D84" s="10"/>
       <c r="E84"/>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>139</v>
-      </c>
-      <c r="C85" s="10" t="s">
-        <v>54</v>
+        <v>144</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="D85" s="10"/>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>140</v>
-      </c>
-      <c r="C86" s="10" t="b">
+        <v>145</v>
+      </c>
+      <c r="C86" s="12" t="b">
         <v>1</v>
       </c>
       <c r="D86" s="10"/>
@@ -2496,7 +2555,7 @@
   <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2522,826 +2581,826 @@
         <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5">
-      <c r="A3" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="18"/>
+      <c r="A3" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:6" ht="16.5">
-      <c r="A4" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="18"/>
+      <c r="A4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" ht="16.5">
-      <c r="A5" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="18"/>
+      <c r="A5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" ht="45.75">
-      <c r="A6" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="D6" s="19" t="s">
+      <c r="A6" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:6" ht="16.5">
+      <c r="A7" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="18"/>
-    </row>
-    <row r="7" spans="1:6" ht="16.5">
-      <c r="A7" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>149</v>
+      </c>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:6" ht="16.5">
+      <c r="A8" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:6" ht="16.5">
+      <c r="A15" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6" ht="30.75">
+      <c r="A18" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6" ht="16.5">
+      <c r="A19" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" ht="16.5">
+      <c r="A20" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="15"/>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="1:6" ht="30.75">
+      <c r="A21" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="1:6" ht="16.5">
+      <c r="A22" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="15"/>
+      <c r="F22" s="14"/>
+    </row>
+    <row r="23" spans="1:6" ht="16.5">
+      <c r="A23" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="15"/>
+      <c r="F23" s="14"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" spans="1:6" ht="16.5">
+      <c r="A27" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="15"/>
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" spans="1:6" ht="16.5">
+      <c r="A28" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="15"/>
+      <c r="F28" s="14"/>
+    </row>
+    <row r="29" spans="1:6" ht="16.5">
+      <c r="A29" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="15"/>
+      <c r="F29" s="14"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="14"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="14"/>
+    </row>
+    <row r="32" spans="1:6" ht="16.5">
+      <c r="A32" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F32" s="14"/>
+    </row>
+    <row r="33" spans="1:6" ht="33">
+      <c r="A33" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B33" s="14"/>
+      <c r="C33" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D33" s="15"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B35" s="14"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+    </row>
+    <row r="36" spans="1:6" ht="16.5">
+      <c r="A36" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B36" s="14"/>
+      <c r="C36" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E7" t="s">
-        <v>144</v>
-      </c>
-      <c r="F7" s="18"/>
-    </row>
-    <row r="8" spans="1:6" ht="16.5">
-      <c r="A8" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="18"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="18"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="18"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="18"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="18"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="18"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="18"/>
-    </row>
-    <row r="15" spans="1:6" ht="16.5">
-      <c r="A15" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="D15" s="19" t="s">
+      <c r="D36" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B37" s="14"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B38" s="14"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="B39" s="14"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+    </row>
+    <row r="41" spans="1:6" ht="16.5">
+      <c r="A41" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B41" s="14"/>
+      <c r="C41" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="18"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="18"/>
-    </row>
-    <row r="18" spans="1:6" ht="30.75">
-      <c r="A18" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="18"/>
-    </row>
-    <row r="19" spans="1:6" ht="16.5">
-      <c r="A19" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="18"/>
-    </row>
-    <row r="20" spans="1:6" ht="16.5">
-      <c r="A20" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="18"/>
-    </row>
-    <row r="21" spans="1:6" ht="30.75">
-      <c r="A21" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="18"/>
-    </row>
-    <row r="22" spans="1:6" ht="16.5">
-      <c r="A22" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="18"/>
-    </row>
-    <row r="23" spans="1:6" ht="16.5">
-      <c r="A23" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="18"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="18"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="18"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="18"/>
-    </row>
-    <row r="27" spans="1:6" ht="16.5">
-      <c r="A27" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="18"/>
-    </row>
-    <row r="28" spans="1:6" ht="16.5">
-      <c r="A28" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="18"/>
-    </row>
-    <row r="29" spans="1:6" ht="16.5">
-      <c r="A29" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="19"/>
-      <c r="F29" s="18"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="18"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="18"/>
-    </row>
-    <row r="32" spans="1:6" ht="16.5">
-      <c r="A32" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="F32" s="18"/>
-    </row>
-    <row r="33" spans="1:6" ht="33">
-      <c r="A33" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-    </row>
-    <row r="36" spans="1:6" ht="16.5">
-      <c r="A36" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-    </row>
-    <row r="41" spans="1:6" ht="16.5">
-      <c r="A41" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E41" s="19"/>
-      <c r="F41" s="18"/>
+      <c r="D41" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="15"/>
+      <c r="F41" s="14"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="18"/>
+      <c r="A42" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="B42" s="14"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="14"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="18"/>
+      <c r="A43" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B43" s="14"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="14"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="18"/>
+      <c r="A44" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="B44" s="14"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="14"/>
     </row>
     <row r="45" spans="1:6" ht="16.5">
-      <c r="A45" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E45" s="19"/>
-      <c r="F45" s="18"/>
+      <c r="A45" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B45" s="14"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="15"/>
+      <c r="F45" s="14"/>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="18"/>
+      <c r="A46" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="B46" s="14"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="14"/>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="18"/>
+      <c r="A47" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B47" s="14"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="14"/>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="B48" s="14"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="14"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="B49" s="14"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="14"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B50" s="14"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="14"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="B51" s="14"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="14"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="B52" s="14"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="14"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B53" s="14"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="14"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="B54" s="14"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="14"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B55" s="14"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="14"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B56" s="14"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="14"/>
+    </row>
+    <row r="57" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A57" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B57" s="14"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="14"/>
+    </row>
+    <row r="58" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A58" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B58" s="14"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="14"/>
+    </row>
+    <row r="59" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A59" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="B59" s="14"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="14"/>
+    </row>
+    <row r="60" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A60" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="B60" s="14"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60" s="15"/>
+      <c r="F60" s="14"/>
+    </row>
+    <row r="61" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A61" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="B61" s="14"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="14"/>
+    </row>
+    <row r="62" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A62" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B62" s="14"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="14"/>
+    </row>
+    <row r="63" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A63" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="B63" s="14"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63" s="15"/>
+      <c r="F63" s="14"/>
+    </row>
+    <row r="64" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A64" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="18"/>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="18"/>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="18"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="18"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="B52" s="18"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="18"/>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="18"/>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="B54" s="18"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="18"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="B55" s="18"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="18"/>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="18" t="s">
+      <c r="B64" s="14"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="14"/>
+    </row>
+    <row r="65" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A65" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="B56" s="18"/>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="18"/>
-    </row>
-    <row r="57" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A57" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="B57" s="18"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="18"/>
-    </row>
-    <row r="58" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A58" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="B58" s="18"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="18"/>
-    </row>
-    <row r="59" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A59" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="B59" s="18"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="18"/>
-    </row>
-    <row r="60" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A60" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="B60" s="18"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E60" s="19"/>
-      <c r="F60" s="18"/>
-    </row>
-    <row r="61" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A61" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="B61" s="18"/>
-      <c r="C61" s="19"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="18"/>
-    </row>
-    <row r="62" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A62" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="B62" s="18"/>
-      <c r="C62" s="19"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="18"/>
-    </row>
-    <row r="63" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A63" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="B63" s="18"/>
-      <c r="C63" s="19"/>
-      <c r="D63" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E63" s="19"/>
-      <c r="F63" s="18"/>
-    </row>
-    <row r="64" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A64" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="B64" s="18"/>
-      <c r="C64" s="19"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="18"/>
-    </row>
-    <row r="65" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A65" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="B65" s="18"/>
-      <c r="C65" s="19"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="18"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="14"/>
     </row>
     <row r="66" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A66" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="B66" s="18"/>
-      <c r="C66" s="19"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="18" t="s">
-        <v>205</v>
+      <c r="A66" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="B66" s="14"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="14" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A67" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="18" t="s">
-        <v>207</v>
+      <c r="A67" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="14" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A68" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="B68" s="18"/>
-      <c r="C68" s="19"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="18"/>
+      <c r="A68" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="B68" s="14"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="14"/>
     </row>
     <row r="69" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A69" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="B69" s="18"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="18"/>
+      <c r="A69" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="B69" s="14"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="14"/>
     </row>
     <row r="70" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A70" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="B70" s="18"/>
-      <c r="C70" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="D70" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E70" s="19"/>
-      <c r="F70" s="18"/>
+      <c r="A70" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B70" s="14"/>
+      <c r="C70" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E70" s="15"/>
+      <c r="F70" s="14"/>
     </row>
     <row r="71" spans="1:6" ht="16.5">
-      <c r="A71" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="B71" s="18"/>
-      <c r="C71" s="19" t="s">
-        <v>213</v>
-      </c>
-      <c r="D71" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E71" s="19"/>
-      <c r="F71" s="18"/>
+      <c r="A71" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="B71" s="14"/>
+      <c r="C71" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E71" s="15"/>
+      <c r="F71" s="14"/>
     </row>
     <row r="72" spans="1:6" ht="16.5">
-      <c r="A72" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="B72" s="18"/>
-      <c r="C72" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="D72" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E72" s="19"/>
-      <c r="F72" s="18"/>
+      <c r="A72" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="B72" s="14"/>
+      <c r="C72" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E72" s="15"/>
+      <c r="F72" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3357,10 +3416,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3370,9 +3429,10 @@
     <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" customWidth="1"/>
     <col min="5" max="5" width="66.42578125" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" ht="24.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -3383,203 +3443,221 @@
         <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="30.75">
+    <row r="6" spans="1:6" ht="30.75">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>149</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="30.75">
+    <row r="11" spans="1:6" ht="30.75">
       <c r="A11" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>227</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="30.75">
+    <row r="14" spans="1:6" ht="30.75">
       <c r="A14" s="1" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30.75">
+        <v>233</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30.75">
       <c r="A15" s="1" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>236</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="D19" s="14"/>
-    </row>
-    <row r="20" spans="1:5">
+        <v>159</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="D19" s="13"/>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="45.75">
       <c r="A21" s="1" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>178</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -3587,23 +3665,23 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -3611,22 +3689,22 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="A26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6">
       <c r="A28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -3642,21 +3720,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.5703125" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="4" width="65.7109375" customWidth="1"/>
+    <col min="3" max="3" width="65.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="52.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -3667,255 +3747,264 @@
         <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="30.75">
+    <row r="3" spans="1:6" ht="30.75">
       <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>238</v>
+        <v>46</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>247</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45.75">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45.75">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>251</v>
+      </c>
+      <c r="F5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30.75">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30.75">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>149</v>
+      </c>
+      <c r="F8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C12" s="14"/>
-    </row>
-    <row r="13" spans="1:5">
+        <v>88</v>
+      </c>
+      <c r="C12" s="13"/>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>246</v>
+        <v>97</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>257</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C14" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="B18" t="s">
-        <v>249</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>250</v>
+        <v>260</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>261</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="C19" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="C20" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C21" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C23" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C24" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C25" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="C26" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="D26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -3928,21 +4017,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA13252-6CA5-4CF2-8825-CD2240AA12A2}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
     <col min="2" max="2" width="37" customWidth="1"/>
-    <col min="3" max="4" width="46.7109375" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="77.42578125" customWidth="1"/>
+    <col min="6" max="6" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -3953,191 +4044,203 @@
         <v>8</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>262</v>
+        <v>273</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
       <c r="E5" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>275</v>
+      </c>
+      <c r="F5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30.75">
+        <v>149</v>
+      </c>
+      <c r="F7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30.75">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C8" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>278</v>
+      </c>
+      <c r="C10" t="s">
+        <v>279</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>280</v>
+      </c>
+      <c r="C11" t="s">
+        <v>281</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>282</v>
+      </c>
+      <c r="C14" t="s">
+        <v>283</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>262</v>
+      </c>
+      <c r="C15" t="s">
+        <v>285</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
         <v>265</v>
       </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>267</v>
-      </c>
-      <c r="C10" t="s">
-        <v>268</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C11" t="s">
-        <v>270</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>271</v>
-      </c>
-      <c r="C14" t="s">
-        <v>272</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>251</v>
-      </c>
-      <c r="C15" t="s">
-        <v>274</v>
-      </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>254</v>
-      </c>
       <c r="C16" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>276</v>
+        <v>287</v>
       </c>
       <c r="C17" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C18" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="75.75" customHeight="1">
       <c r="A20" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>173</v>
+        <v>178</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>